<commit_message>
program with serializer updated
</commit_message>
<xml_diff>
--- a/Dashboard/media/out.xlsx
+++ b/Dashboard/media/out.xlsx
@@ -1311,13 +1311,13 @@
         </is>
       </c>
       <c r="C5" s="25" t="n">
-        <v>22</v>
+        <v>100000</v>
       </c>
       <c r="D5" s="25" t="n">
         <v>82</v>
       </c>
       <c r="E5" s="25" t="n">
-        <v>0</v>
+        <v>299</v>
       </c>
       <c r="F5" s="25" t="n">
         <v>6967</v>
@@ -1449,7 +1449,7 @@
         <v>90</v>
       </c>
       <c r="E6" s="25" t="n">
-        <v>0</v>
+        <v>281</v>
       </c>
       <c r="F6" s="25" t="n">
         <v>0</v>
@@ -1581,7 +1581,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="25" t="n">
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="F7" s="25" t="n">
         <v>0</v>
@@ -1713,7 +1713,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="25" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F8" s="25" t="n">
         <v>0</v>
@@ -1845,7 +1845,7 @@
         <v>40</v>
       </c>
       <c r="E9" s="25" t="n">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="F9" s="25" t="n">
         <v>10</v>
@@ -1977,7 +1977,7 @@
         <v>18</v>
       </c>
       <c r="E10" s="25" t="n">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="F10" s="25" t="n">
         <v>0</v>
@@ -2107,7 +2107,7 @@
         <v>4</v>
       </c>
       <c r="E11" s="25" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="F11" s="25" t="n">
         <v>0</v>
@@ -2237,7 +2237,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="25" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F12" s="25" t="n">
         <v>0</v>
@@ -2367,7 +2367,7 @@
         <v>14</v>
       </c>
       <c r="E13" s="25" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="F13" s="25" t="n">
         <v>0</v>
@@ -2499,7 +2499,7 @@
         <v>45</v>
       </c>
       <c r="E14" s="25" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F14" s="25" t="n">
         <v>-10</v>
@@ -2625,13 +2625,13 @@
         </is>
       </c>
       <c r="C15" s="27" t="n">
-        <v>2999</v>
+        <v>0</v>
       </c>
       <c r="D15" s="27" t="n">
         <v>10</v>
       </c>
       <c r="E15" s="28" t="n">
-        <v>0</v>
+        <v>289</v>
       </c>
       <c r="F15" s="28" t="n">
         <v>0</v>
@@ -2889,13 +2889,13 @@
         </is>
       </c>
       <c r="C17" s="27" t="n">
-        <v>2999</v>
+        <v>0</v>
       </c>
       <c r="D17" s="27" t="n">
         <v>8</v>
       </c>
       <c r="E17" s="27" t="n">
-        <v>0</v>
+        <v>289</v>
       </c>
       <c r="F17" s="27" t="n">
         <v>0</v>
@@ -3021,13 +3021,13 @@
         </is>
       </c>
       <c r="C18" s="25" t="n">
-        <v>-2999</v>
+        <v>0</v>
       </c>
       <c r="D18" s="25" t="n">
         <v>37</v>
       </c>
       <c r="E18" s="25" t="n">
-        <v>0</v>
+        <v>-286</v>
       </c>
       <c r="F18" s="25" t="n">
         <v>-10</v>
@@ -3159,7 +3159,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="25" t="n">
-        <v>0</v>
+        <v>3.2</v>
       </c>
       <c r="F19" s="25" t="n">
         <v>0</v>
@@ -3291,7 +3291,7 @@
         <v>20</v>
       </c>
       <c r="E20" s="25" t="n">
-        <v>0</v>
+        <v>30.25</v>
       </c>
       <c r="F20" s="25" t="n">
         <v>0</v>
@@ -3423,7 +3423,7 @@
         <v>50</v>
       </c>
       <c r="E21" s="25" t="n">
-        <v>0</v>
+        <v>1.07</v>
       </c>
       <c r="F21" s="25" t="n">
         <v>0</v>
@@ -3555,7 +3555,7 @@
         <v>17.78</v>
       </c>
       <c r="E22" s="25" t="n">
-        <v>0</v>
+        <v>9633.33</v>
       </c>
       <c r="F22" s="25" t="n">
         <v>-0</v>
@@ -3687,7 +3687,7 @@
         <v>82.22</v>
       </c>
       <c r="E23" s="25" t="n">
-        <v>0</v>
+        <v>-9533.33</v>
       </c>
       <c r="F23" s="25" t="n">
         <v>100</v>
@@ -3859,13 +3859,13 @@
         </is>
       </c>
       <c r="C25" s="25" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D25" s="25" t="n">
         <v>8</v>
       </c>
       <c r="E25" s="25" t="n">
-        <v>10</v>
+        <v>3.25</v>
       </c>
       <c r="F25" s="25" t="n">
         <v>32.2</v>
@@ -3989,13 +3989,13 @@
         </is>
       </c>
       <c r="C26" s="25" t="n">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="D26" s="25" t="n">
         <v>3.36</v>
       </c>
       <c r="E26" s="25" t="n">
-        <v>10.1</v>
+        <v>3.25</v>
       </c>
       <c r="F26" s="25" t="n">
         <v>12.2</v>
@@ -4119,13 +4119,13 @@
         </is>
       </c>
       <c r="C27" s="25" t="n">
-        <v>20.1</v>
+        <v>0</v>
       </c>
       <c r="D27" s="25" t="n">
         <v>5.25</v>
       </c>
       <c r="E27" s="25" t="n">
-        <v>10.2</v>
+        <v>3.25</v>
       </c>
       <c r="F27" s="25" t="n">
         <v>3</v>

</xml_diff>